<commit_message>
Mostly adding the excel doc
</commit_message>
<xml_diff>
--- a/VSTips.xlsx
+++ b/VSTips.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\VSTips\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907B6942-A5EE-4519-BD32-10B5D0861064}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC168CF-2B68-47BC-8F16-8238CD2A796B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{45FA8023-CE65-4427-B3AD-1FEDBC78C3D5}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="154">
   <si>
     <t>Category</t>
   </si>
@@ -489,13 +488,19 @@
   </si>
   <si>
     <t>https://hutchcodes.net/2019/04/visual-studio-tips-editing-shortcuts/</t>
+  </si>
+  <si>
+    <t>https://hutchcodes.net/2019/04/visual-studio-tips-code-definition-keyboard-shortcuts/</t>
+  </si>
+  <si>
+    <t>https://hutchcodes.net/2019/04/visual-studio-tips-test-explorer/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -511,13 +516,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -529,15 +546,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -853,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB29BD7D-6726-4C8F-9E83-B7576FA94D25}">
   <dimension ref="A1:F110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="K87" sqref="K87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1346,6 +1366,9 @@
       <c r="C36" t="s">
         <v>48</v>
       </c>
+      <c r="D36" s="1" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -1357,6 +1380,9 @@
       <c r="C37" t="s">
         <v>49</v>
       </c>
+      <c r="D37" s="1" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -1368,6 +1394,9 @@
       <c r="C38" t="s">
         <v>50</v>
       </c>
+      <c r="D38" s="1" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -1379,6 +1408,9 @@
       <c r="C39" t="s">
         <v>51</v>
       </c>
+      <c r="D39" s="1" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -1390,6 +1422,9 @@
       <c r="C40" t="s">
         <v>52</v>
       </c>
+      <c r="D40" s="1" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -1834,6 +1869,9 @@
       <c r="C85" t="s">
         <v>104</v>
       </c>
+      <c r="D85" s="1" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
@@ -1842,6 +1880,9 @@
       <c r="C86" t="s">
         <v>105</v>
       </c>
+      <c r="D86" s="1" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
@@ -1850,6 +1891,9 @@
       <c r="C87" t="s">
         <v>106</v>
       </c>
+      <c r="D87" s="1" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
@@ -1858,16 +1902,22 @@
       <c r="C88" t="s">
         <v>107</v>
       </c>
+      <c r="D88" s="1" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>108</v>
       </c>
       <c r="B89" t="s">
-        <v>23</v>
+        <v>115</v>
       </c>
       <c r="C89" t="s">
-        <v>110</v>
+        <v>34</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -1878,7 +1928,7 @@
         <v>115</v>
       </c>
       <c r="C90" t="s">
-        <v>34</v>
+        <v>109</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>146</v>
@@ -1892,101 +1942,98 @@
         <v>115</v>
       </c>
       <c r="C91" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+    <row r="92" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B92" t="s">
-        <v>115</v>
-      </c>
-      <c r="C92" t="s">
-        <v>116</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+      <c r="B92" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C93" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+      <c r="C93" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C94" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+      <c r="C94" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C95" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+      <c r="C95" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C96" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="C96" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C97" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="C97" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C98" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+      <c r="C98" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C99" t="s">
-        <v>109</v>
+      <c r="C99" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -2098,13 +2145,22 @@
     <hyperlink ref="D24" r:id="rId14" xr:uid="{FF210229-E9F2-40DC-8E3B-28A38487074C}"/>
     <hyperlink ref="D25" r:id="rId15" xr:uid="{4A1C4B99-BE60-4295-AFF4-F6C6B2FBADE5}"/>
     <hyperlink ref="D15" r:id="rId16" xr:uid="{BC4726A8-5BFC-4ECA-A118-8921DEA4B96D}"/>
-    <hyperlink ref="D90" r:id="rId17" xr:uid="{67D98544-561A-48F2-8291-3C7285728DF0}"/>
-    <hyperlink ref="D91" r:id="rId18" xr:uid="{4CD5C3C4-5DF5-462C-AFDE-BC546F47AB36}"/>
-    <hyperlink ref="D92" r:id="rId19" xr:uid="{DBB925CD-8202-419E-85DB-987D891CD62B}"/>
+    <hyperlink ref="D89" r:id="rId17" xr:uid="{67D98544-561A-48F2-8291-3C7285728DF0}"/>
+    <hyperlink ref="D90" r:id="rId18" xr:uid="{4CD5C3C4-5DF5-462C-AFDE-BC546F47AB36}"/>
+    <hyperlink ref="D91" r:id="rId19" xr:uid="{DBB925CD-8202-419E-85DB-987D891CD62B}"/>
     <hyperlink ref="D69" r:id="rId20" xr:uid="{61D2E5AB-4958-479E-B43D-C325680815A0}"/>
+    <hyperlink ref="D36" r:id="rId21" xr:uid="{BDD45BB3-3B69-417A-8238-767B14A156AB}"/>
+    <hyperlink ref="D37" r:id="rId22" xr:uid="{7A250956-FDF5-4776-8C3B-2A6E2421EE31}"/>
+    <hyperlink ref="D38" r:id="rId23" xr:uid="{40C2E3EC-18AE-4115-863B-B92F9FAAB437}"/>
+    <hyperlink ref="D39" r:id="rId24" xr:uid="{FE354835-622A-4AC0-ACED-BDA5635CA872}"/>
+    <hyperlink ref="D40" r:id="rId25" xr:uid="{3CB25463-CB93-47C9-A358-7F9BCC9DBEF0}"/>
+    <hyperlink ref="D85" r:id="rId26" xr:uid="{B3975BB8-E879-4F99-9565-FFD111C30916}"/>
+    <hyperlink ref="D86" r:id="rId27" xr:uid="{540B0A5F-E844-4FE2-B9CE-BAA6C4F55AE4}"/>
+    <hyperlink ref="D87" r:id="rId28" xr:uid="{C6885693-D0C8-4EEA-86D4-39A8EB671C87}"/>
+    <hyperlink ref="D88" r:id="rId29" xr:uid="{C27506E6-B2B7-4231-AC2C-47BE3278ACC8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId21"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId30"/>
 </worksheet>
 </file>
 

</xml_diff>